<commit_message>
changement: page2 - titre - descriotion - balise inu - lien footer - nav contact -lang
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicopatsch/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexweinachter/Desktop/projet4/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1912D41C-98FC-834E-8827-AB0D9E6E71DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="620" windowWidth="27860" windowHeight="17380" tabRatio="500"/>
+    <workbookView xWindow="940" yWindow="500" windowWidth="27860" windowHeight="16360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Catégorie</t>
   </si>
@@ -51,12 +52,81 @@
   </si>
   <si>
     <t>(SEO ou accessiblité ?)</t>
+  </si>
+  <si>
+    <t>page2.html</t>
+  </si>
+  <si>
+    <t>pas de description</t>
+  </si>
+  <si>
+    <t>1 balise li inutile</t>
+  </si>
+  <si>
+    <t>toggle navigation sans icone page2</t>
+  </si>
+  <si>
+    <t>texte trop petit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">balise meta keyword </t>
+  </si>
+  <si>
+    <t>html lang = default</t>
+  </si>
+  <si>
+    <t>trop de lien dans le footer (crawlabilité)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minifiez et compressez Js et css </t>
+  </si>
+  <si>
+    <t>taille image</t>
+  </si>
+  <si>
+    <t>text format image (avis)</t>
+  </si>
+  <si>
+    <t>formulaire de contact</t>
+  </si>
+  <si>
+    <t>ressource async / defer manquante sur le script Js</t>
+  </si>
+  <si>
+    <t>fait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fait </t>
+  </si>
+  <si>
+    <t>contact.html</t>
+  </si>
+  <si>
+    <t>lang = fr</t>
+  </si>
+  <si>
+    <t>ajout description avec mot clef</t>
+  </si>
+  <si>
+    <t>supp</t>
+  </si>
+  <si>
+    <t>pas de titre de page et titre page2</t>
+  </si>
+  <si>
+    <t>agance la panthere et Contact</t>
+  </si>
+  <si>
+    <t>supp toggle + 1partie du menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">partie responsive nul ( text et formulaire)et ajuster css </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -139,6 +209,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -341,16 +414,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="4" max="4" width="40.85546875" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
     <col min="6" max="6" width="21.28515625" customWidth="1"/>
     <col min="7" max="26" width="10.5703125" customWidth="1"/>
@@ -403,61 +479,149 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
       <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
       <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1425,7 +1589,6 @@
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
description image, changer paris, text en format img
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexweinachter/Desktop/projet4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECAEA43-C276-6B48-BE43-BE14E2983FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B5CDE5-7864-A144-B581-9D94D85C5E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="500" windowWidth="27860" windowHeight="16340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Catégorie</t>
   </si>
@@ -84,9 +84,6 @@
     <t>taille image</t>
   </si>
   <si>
-    <t>text format image (avis)</t>
-  </si>
-  <si>
     <t>formulaire de contact</t>
   </si>
   <si>
@@ -126,7 +123,25 @@
     <t xml:space="preserve">paris </t>
   </si>
   <si>
-    <t xml:space="preserve">couleur </t>
+    <t>couleur et contraste</t>
+  </si>
+  <si>
+    <t>changer</t>
+  </si>
+  <si>
+    <t>description image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text format image </t>
+  </si>
+  <si>
+    <t>text à la place d'image</t>
+  </si>
+  <si>
+    <t>remplacer lyon par paris</t>
+  </si>
+  <si>
+    <t>modifier</t>
   </si>
 </sst>
 </file>
@@ -423,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -489,22 +504,22 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
       </c>
       <c r="E4" s="4"/>
     </row>
@@ -513,10 +528,10 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="4"/>
     </row>
@@ -525,10 +540,10 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="4"/>
     </row>
@@ -537,10 +552,10 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="4"/>
     </row>
@@ -549,10 +564,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="4"/>
     </row>
@@ -566,6 +581,12 @@
       <c r="B10" t="s">
         <v>12</v>
       </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -573,10 +594,10 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -594,48 +615,70 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>17</v>
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>